<commit_message>
Fix date in changelog
</commit_message>
<xml_diff>
--- a/PNG/tbemr_basicRegister_codebook_v1.6_png.xlsx
+++ b/PNG/tbemr_basicRegister_codebook_v1.6_png.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://msfintl-my.sharepoint.com/personal/kristina_reinhardt_newyork_msf_org/Documents/github/mart-tbemr-query-library/PNG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="13_ncr:1_{53EDD30D-FEC4-4192-ABC0-295A218D3490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38903CED-86E8-45B1-8D2D-17905DC3D01C}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="13_ncr:1_{53EDD30D-FEC4-4192-ABC0-295A218D3490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FEF490C-A1EB-491E-A5FF-BD959BDBB2B1}"/>
   <bookViews>
-    <workbookView xWindow="14505" yWindow="-13500" windowWidth="12000" windowHeight="12900" xr2:uid="{A005DB92-A8DC-40CC-A3FD-38C99E047FDE}"/>
+    <workbookView xWindow="2385" yWindow="-13620" windowWidth="24240" windowHeight="13140" xr2:uid="{A005DB92-A8DC-40CC-A3FD-38C99E047FDE}"/>
   </bookViews>
   <sheets>
     <sheet name="query_changelog" sheetId="2" r:id="rId1"/>
@@ -1315,7 +1315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1378,9 +1378,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1700,7 +1697,7 @@
   <dimension ref="B1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1879,7 +1876,7 @@
     </row>
     <row r="17" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B17" s="19">
-        <v>44935</v>
+        <v>44966</v>
       </c>
       <c r="C17" s="20" t="s">
         <v>315</v>
@@ -2379,7 +2376,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="2" t="s">
         <v>261</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -2408,7 +2405,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" s="2" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="2" t="s">
         <v>262</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -4173,18 +4170,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4397,18 +4394,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEAC8D0C-DBC1-4884-B9C9-C3DF8114B459}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{357647DF-603C-4CA9-B082-BB6ADB1E29DD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{357647DF-603C-4CA9-B082-BB6ADB1E29DD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEAC8D0C-DBC1-4884-B9C9-C3DF8114B459}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>